<commit_message>
Add last update data to editlist.xlsx
</commit_message>
<xml_diff>
--- a/edit_list.xlsx
+++ b/edit_list.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>journal</t>
   </si>
@@ -66,6 +66,9 @@
   </si>
   <si>
     <t>http://pps.sagepub.com/content/[0-9]{1,}/[0-9]{1,}/[0-9]{1,}.abstract</t>
+  </si>
+  <si>
+    <t>update</t>
   </si>
 </sst>
 </file>
@@ -426,77 +429,86 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" customWidth="1"/>
-    <col min="3" max="3" width="16.42578125" customWidth="1"/>
-    <col min="4" max="5" width="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" customWidth="1"/>
+    <col min="4" max="4" width="16.42578125" customWidth="1"/>
+    <col min="5" max="6" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>20150809</v>
+      </c>
+      <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>8</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>20150809</v>
+      </c>
+      <c r="B3" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>14</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1"/>
-    <hyperlink ref="C3" r:id="rId2"/>
-    <hyperlink ref="D3" r:id="rId3"/>
-    <hyperlink ref="E3" r:id="rId4"/>
+    <hyperlink ref="C3" r:id="rId1"/>
+    <hyperlink ref="D3" r:id="rId2"/>
+    <hyperlink ref="E3" r:id="rId3"/>
+    <hyperlink ref="F3" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>

</xml_diff>

<commit_message>
Add and test perspsocialpsychrev
</commit_message>
<xml_diff>
--- a/edit_list.xlsx
+++ b/edit_list.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>journal</t>
   </si>
@@ -69,6 +69,21 @@
   </si>
   <si>
     <t>update</t>
+  </si>
+  <si>
+    <t>perssocialpsychrev</t>
+  </si>
+  <si>
+    <t>http://psr.sagepub.com/content/by/year/</t>
+  </si>
+  <si>
+    <t>http://psr.sagepub.com/content/by/year/[0-9]{4}</t>
+  </si>
+  <si>
+    <t>http://psr.sagepub.com/content/vol[0-9]{1,}/issue[0-9]{1,}/</t>
+  </si>
+  <si>
+    <t>http://psr.sagepub.com/content/[0-9]{1,}/[0-9]{1,}/[0-9]{1,}.abstract</t>
   </si>
 </sst>
 </file>
@@ -429,10 +444,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -503,12 +518,32 @@
         <v>14</v>
       </c>
     </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>20150809</v>
+      </c>
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" t="s">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C3" r:id="rId1"/>
-    <hyperlink ref="D3" r:id="rId2"/>
-    <hyperlink ref="E3" r:id="rId3"/>
-    <hyperlink ref="F3" r:id="rId4"/>
+    <hyperlink ref="F3" r:id="rId1"/>
+    <hyperlink ref="E3" r:id="rId2"/>
+    <hyperlink ref="D3" r:id="rId3"/>
+    <hyperlink ref="C3" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>

</xml_diff>

<commit_message>
Add publisher to editlist
</commit_message>
<xml_diff>
--- a/edit_list.xlsx
+++ b/edit_list.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
   <si>
     <t>journal</t>
   </si>
@@ -84,6 +84,12 @@
   </si>
   <si>
     <t>http://psr.sagepub.com/content/[0-9]{1,}/[0-9]{1,}/[0-9]{1,}.abstract</t>
+  </si>
+  <si>
+    <t>publisher</t>
+  </si>
+  <si>
+    <t>sage</t>
   </si>
 </sst>
 </file>
@@ -444,106 +450,118 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.85546875" customWidth="1"/>
-    <col min="4" max="4" width="16.42578125" customWidth="1"/>
-    <col min="5" max="6" width="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.85546875" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" customWidth="1"/>
+    <col min="6" max="7" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>20150809</v>
       </c>
       <c r="B2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>7</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>8</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>20150809</v>
       </c>
       <c r="B3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="G3" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>20150809</v>
       </c>
       <c r="B4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" t="s">
         <v>16</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>17</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>18</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>19</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>20</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F3" r:id="rId1"/>
-    <hyperlink ref="E3" r:id="rId2"/>
-    <hyperlink ref="D3" r:id="rId3"/>
-    <hyperlink ref="C3" r:id="rId4"/>
+    <hyperlink ref="G3" r:id="rId1"/>
+    <hyperlink ref="F3" r:id="rId2"/>
+    <hyperlink ref="E3" r:id="rId3"/>
+    <hyperlink ref="D3" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>

</xml_diff>